<commit_message>
Erste Teile des Klassenkonferenzprotokolls werden geschrieben.
</commit_message>
<xml_diff>
--- a/data/Sitzungsleiter.xlsx
+++ b/data/Sitzungsleiter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Klasse</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>15:00</t>
+  </si>
+  <si>
+    <t>05D</t>
+  </si>
+  <si>
+    <t>05E</t>
+  </si>
+  <si>
+    <t>05F</t>
+  </si>
+  <si>
+    <t>05G</t>
   </si>
 </sst>
 </file>
@@ -410,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,6 +505,74 @@
         <v>13</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Erste komplett lauffähige und grob getestete Version.
</commit_message>
<xml_diff>
--- a/data/Sitzungsleiter.xlsx
+++ b/data/Sitzungsleiter.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="44">
   <si>
     <t>Klasse</t>
   </si>
@@ -71,6 +71,81 @@
   </si>
   <si>
     <t>05G</t>
+  </si>
+  <si>
+    <t>06A</t>
+  </si>
+  <si>
+    <t>06B</t>
+  </si>
+  <si>
+    <t>06C</t>
+  </si>
+  <si>
+    <t>06D</t>
+  </si>
+  <si>
+    <t>06E</t>
+  </si>
+  <si>
+    <t>07A</t>
+  </si>
+  <si>
+    <t>07B</t>
+  </si>
+  <si>
+    <t>07C</t>
+  </si>
+  <si>
+    <t>07D</t>
+  </si>
+  <si>
+    <t>08A</t>
+  </si>
+  <si>
+    <t>08B</t>
+  </si>
+  <si>
+    <t>08C</t>
+  </si>
+  <si>
+    <t>08D</t>
+  </si>
+  <si>
+    <t>09A</t>
+  </si>
+  <si>
+    <t>09B</t>
+  </si>
+  <si>
+    <t>09C</t>
+  </si>
+  <si>
+    <t>09D</t>
+  </si>
+  <si>
+    <t>10A</t>
+  </si>
+  <si>
+    <t>10B</t>
+  </si>
+  <si>
+    <t>10C</t>
+  </si>
+  <si>
+    <t>10D</t>
+  </si>
+  <si>
+    <t>Livia Schleßing, OStRin</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>07E</t>
+  </si>
+  <si>
+    <t>07F</t>
   </si>
 </sst>
 </file>
@@ -422,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -573,6 +648,397 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Funktionalitäten fürs Jahreszeugnis in eigenes Package verlagert
</commit_message>
<xml_diff>
--- a/data/Sitzungsleiter.xlsx
+++ b/data/Sitzungsleiter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sitzungsplan" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="53">
   <si>
     <t>Klasse</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>18:30</t>
+  </si>
+  <si>
+    <t>06F</t>
+  </si>
+  <si>
+    <t>08D</t>
   </si>
 </sst>
 </file>
@@ -518,22 +524,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="2"/>
-    <col min="2" max="2" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -567,7 +573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -584,7 +590,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -601,7 +607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -618,7 +624,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -635,7 +641,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -652,7 +658,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -669,7 +675,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -686,7 +692,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -703,7 +709,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -720,7 +726,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -737,7 +743,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -754,114 +760,114 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>12</v>
@@ -873,63 +879,63 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>43</v>
@@ -941,105 +947,139 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated reference to apache pdfbox due to security vulnerability reported from GitHub
</commit_message>
<xml_diff>
--- a/data/Sitzungsleiter.xlsx
+++ b/data/Sitzungsleiter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sitzungsplan" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>05C</t>
   </si>
   <si>
-    <t>Gerhard Maier, OStD</t>
-  </si>
-  <si>
     <t>Datum</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>10D</t>
   </si>
   <si>
-    <t>Livia Schleßing, OStRin</t>
-  </si>
-  <si>
     <t>15:30</t>
   </si>
   <si>
@@ -154,7 +148,13 @@
     <t>08D</t>
   </si>
   <si>
-    <t>19.02.2018</t>
+    <t>Iris Jamnitzky, OStDin</t>
+  </si>
+  <si>
+    <t>17.07.2018</t>
+  </si>
+  <si>
+    <t>Livia Schleßing, StDin</t>
   </si>
 </sst>
 </file>
@@ -509,19 +509,19 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,44 +535,44 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -580,404 +580,404 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>